<commit_message>
30.11.2021 Capital Statement Info
</commit_message>
<xml_diff>
--- a/Realme/Others/Realme DOA+Servicing  Sheet.xlsx
+++ b/Realme/Others/Realme DOA+Servicing  Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>S.N</t>
   </si>
@@ -89,6 +89,33 @@
   </si>
   <si>
     <t xml:space="preserve">1 time 20days stay in CC. 2nd Time same problem </t>
+  </si>
+  <si>
+    <t>Desh mobile</t>
+  </si>
+  <si>
+    <t>c25s-128</t>
+  </si>
+  <si>
+    <t>30.11.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shohan enterprise </t>
+  </si>
+  <si>
+    <t>Apurbo mobile</t>
+  </si>
+  <si>
+    <t>c20a</t>
+  </si>
+  <si>
+    <t>friends mobile</t>
+  </si>
+  <si>
+    <t>P+C</t>
+  </si>
+  <si>
+    <t>C25s/64</t>
   </si>
 </sst>
 </file>
@@ -546,7 +573,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,19 +653,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4">
-        <v>868529041973511</v>
+        <v>867623053838711</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -647,19 +674,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4">
-        <v>869092052372098</v>
+        <v>869092052729339</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -668,19 +695,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4">
-        <v>867623051022870</v>
+        <v>868790052445811</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -688,22 +715,42 @@
       <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="5"/>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4">
+        <v>864623050833338</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="5"/>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4">
+        <v>867623050430934</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>